<commit_message>
Contains a key required in process
Notepad file path key
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,15 @@
     <t>Static part of logging message. Processed Transaction failed with application exception.</t>
   </si>
   <si>
+    <t>Notepad_Execution_File</t>
+  </si>
+  <si>
+    <t>C:\Windows\System32\notepad.exe</t>
+  </si>
+  <si>
+    <t>Path to Notepad Execution File</t>
+  </si>
+  <si>
     <t>Asset</t>
   </si>
   <si>
@@ -112,7 +121,7 @@
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,38 +137,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -170,16 +150,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,37 +173,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,8 +212,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,18 +264,26 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -293,13 +296,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,49 +344,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,97 +380,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,6 +402,84 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -484,80 +487,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -580,6 +509,80 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -587,159 +590,155 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1063,7 +1062,7 @@
   <sheetPr/>
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1109,11 +1108,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-    </row>
+    <row r="2" ht="14.25" customHeight="1"/>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="28.8" spans="1:3">
       <c r="A4" t="s">
@@ -1122,7 +1117,7 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2131,8 +2126,8 @@
   <sheetPr/>
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4537037037037" defaultRowHeight="15" customHeight="1"/>
@@ -2256,7 +2251,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1" spans="1:3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
@@ -3261,10 +3266,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>